<commit_message>
Updated cleaned Excel dataset for Power BI integration
Reorganized Excel sheet for structured Power BI import

- Added Data Collected column to all overview and data sheets

Utilized PowerQuery in PowerBI for data cleaning and transformation

- Cleaned data types (numbers, percentages)
- Applied conditional logic to separate numeric and percentage metrics
- Removed unnecessary rows (pivot table from Excel)
</commit_message>
<xml_diff>
--- a/ROSÉ Business Insights.xlsx
+++ b/ROSÉ Business Insights.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nzmz_\Desktop\Data Analyst Portfolio\Ros-_Entertainment_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0B9B9A-E049-474A-9337-5DA58AC8B4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A167CE22-586F-463C-9E6C-6DE1FAD5C467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="12" activeTab="16" xr2:uid="{0FA3C6EE-BCC2-4624-8E49-B02A035F49AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="13" xr2:uid="{0FA3C6EE-BCC2-4624-8E49-B02A035F49AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Notes" sheetId="2" r:id="rId1"/>
     <sheet name="Summary" sheetId="1" r:id="rId2"/>
     <sheet name="Spotify" sheetId="3" r:id="rId3"/>
-    <sheet name="SpotifyData_Stats" sheetId="9" r:id="rId4"/>
-    <sheet name="SpotifyData_Tracks" sheetId="10" r:id="rId5"/>
-    <sheet name="SpotifyData_Albums" sheetId="11" r:id="rId6"/>
+    <sheet name="Spotify_Overview" sheetId="9" r:id="rId4"/>
+    <sheet name="Spotify_Tracks" sheetId="10" r:id="rId5"/>
+    <sheet name="Spotify_Albums" sheetId="11" r:id="rId6"/>
     <sheet name="YouTube" sheetId="4" r:id="rId7"/>
-    <sheet name="YouTubeData_Stats" sheetId="12" r:id="rId8"/>
-    <sheet name="YouTubeData_MVs" sheetId="13" r:id="rId9"/>
+    <sheet name="YouTube_Overview" sheetId="12" r:id="rId8"/>
+    <sheet name="YouTube_MVs" sheetId="13" r:id="rId9"/>
     <sheet name="Instagram" sheetId="5" r:id="rId10"/>
-    <sheet name="InstagramData_Stats" sheetId="14" r:id="rId11"/>
-    <sheet name="InstagramData_Posts" sheetId="15" r:id="rId12"/>
+    <sheet name="Instagram_Overview" sheetId="14" r:id="rId11"/>
+    <sheet name="Instagram_Posts" sheetId="15" r:id="rId12"/>
     <sheet name="Twitter_X" sheetId="6" r:id="rId13"/>
-    <sheet name="TwitterData_Stats" sheetId="16" r:id="rId14"/>
-    <sheet name="TwitterData_Tweets" sheetId="17" r:id="rId15"/>
+    <sheet name="Twitter_Overview" sheetId="16" r:id="rId14"/>
+    <sheet name="Twitter_Tweets" sheetId="17" r:id="rId15"/>
     <sheet name="Google Trends" sheetId="7" r:id="rId16"/>
     <sheet name="GoogleTrends_InterestOverTime" sheetId="18" r:id="rId17"/>
     <sheet name="GoogleTrends_InterestOverRegion" sheetId="19" r:id="rId18"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="160">
   <si>
     <t>ROSÉ Entertainment Data</t>
   </si>
@@ -637,13 +637,7 @@
     <t>618,184 listeners</t>
   </si>
   <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
     <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Sum of Stream</t>
   </si>
   <si>
     <t>Follower Count</t>
@@ -887,13 +881,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1156,7 +1150,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Zulaikha Zulasri" refreshedDate="45920.838263078702" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="17" xr:uid="{753EE862-D31A-4654-998A-092F4383BEDC}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E18" sheet="SpotifyData_Tracks"/>
+    <worksheetSource ref="A1:E18" sheet="Spotify_Tracks"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Track Title" numFmtId="0">
@@ -1332,10 +1326,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10202EDA-500A-4C2D-AF0C-71759D0F0112}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10202EDA-500A-4C2D-AF0C-71759D0F0112}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Album Title">
+  <location ref="A1:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField showAll="0">
       <items count="18">
         <item x="10"/>
         <item x="3"/>
@@ -1371,76 +1365,24 @@
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField numFmtId="20" showAll="0"/>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="1">
     <field x="1"/>
-    <field x="0"/>
   </rowFields>
-  <rowItems count="23">
+  <rowItems count="6">
     <i>
       <x/>
-    </i>
-    <i r="1">
-      <x v="7"/>
     </i>
     <i>
       <x v="1"/>
     </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
     <i>
       <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
     </i>
     <i>
       <x v="3"/>
     </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
     <i>
       <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
     </i>
     <i t="grand">
       <x/>
@@ -1450,7 +1392,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Stream" fld="2" baseField="0" baseItem="0" numFmtId="3"/>
+    <dataField name="Total Stream" fld="2" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2499,7 +2441,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2520,7 +2462,7 @@
       <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="34"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2578,10 +2520,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CFEFA5-869B-4A48-85D0-E4B81BA37CC7}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2592,9 +2534,10 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>77</v>
       </c>
@@ -2608,13 +2551,16 @@
         <v>94</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>45913</v>
       </c>
@@ -2628,15 +2574,18 @@
         <v>19100</v>
       </c>
       <c r="E2" s="17">
-        <f>InstagramData_Stats!$B$2</f>
+        <f>Instagram_Overview!$B$2</f>
         <v>84601628</v>
       </c>
       <c r="F2" s="18">
         <f>SUM(C2:D2)/E2</f>
         <v>3.3567592812752962E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>45913</v>
       </c>
@@ -2650,15 +2599,18 @@
         <v>9452</v>
       </c>
       <c r="E3" s="17">
-        <f>InstagramData_Stats!$B$2</f>
+        <f>Instagram_Overview!$B$2</f>
         <v>84601628</v>
       </c>
       <c r="F3" s="18">
         <f t="shared" ref="F3:F11" si="0">SUM(C3:D3)/E3</f>
         <v>6.3051268942484178E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>45913</v>
       </c>
@@ -2672,15 +2624,18 @@
         <v>17400</v>
       </c>
       <c r="E4" s="17">
-        <f>InstagramData_Stats!$B$2</f>
+        <f>Instagram_Overview!$B$2</f>
         <v>84601628</v>
       </c>
       <c r="F4" s="18">
         <f t="shared" si="0"/>
         <v>2.2036112591119403E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>45909</v>
       </c>
@@ -2694,15 +2649,18 @@
         <v>29000</v>
       </c>
       <c r="E5" s="17">
-        <f>InstagramData_Stats!$B$2</f>
+        <f>Instagram_Overview!$B$2</f>
         <v>84601628</v>
       </c>
       <c r="F5" s="18">
         <f t="shared" si="0"/>
         <v>2.8334041042330768E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>45908</v>
       </c>
@@ -2716,15 +2674,18 @@
         <v>20600</v>
       </c>
       <c r="E6" s="17">
-        <f>InstagramData_Stats!$B$2</f>
+        <f>Instagram_Overview!$B$2</f>
         <v>84601628</v>
       </c>
       <c r="F6" s="18">
         <f t="shared" si="0"/>
         <v>3.9236620836658131E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>45900</v>
       </c>
@@ -2738,15 +2699,18 @@
         <v>22200</v>
       </c>
       <c r="E7" s="17">
-        <f>InstagramData_Stats!$B$2</f>
+        <f>Instagram_Overview!$B$2</f>
         <v>84601628</v>
       </c>
       <c r="F7" s="18">
         <f t="shared" si="0"/>
         <v>3.5659786594177595E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>45895</v>
       </c>
@@ -2760,15 +2724,18 @@
         <v>10600</v>
       </c>
       <c r="E8" s="17">
-        <f>InstagramData_Stats!$B$2</f>
+        <f>Instagram_Overview!$B$2</f>
         <v>84601628</v>
       </c>
       <c r="F8" s="18">
         <f t="shared" si="0"/>
         <v>1.6183163756612343E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>45893</v>
       </c>
@@ -2782,15 +2749,18 @@
         <v>12400</v>
       </c>
       <c r="E9" s="17">
-        <f>InstagramData_Stats!$B$2</f>
+        <f>Instagram_Overview!$B$2</f>
         <v>84601628</v>
       </c>
       <c r="F9" s="18">
         <f t="shared" si="0"/>
         <v>2.9737453752072006E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>45887</v>
       </c>
@@ -2804,15 +2774,18 @@
         <v>11000</v>
       </c>
       <c r="E10" s="17">
-        <f>InstagramData_Stats!$B$2</f>
+        <f>Instagram_Overview!$B$2</f>
         <v>84601628</v>
       </c>
       <c r="F10" s="18">
         <f t="shared" si="0"/>
         <v>2.0392704499729013E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>45880</v>
       </c>
@@ -2826,12 +2799,15 @@
         <v>20400</v>
       </c>
       <c r="E11" s="17">
-        <f>InstagramData_Stats!$B$2</f>
+        <f>Instagram_Overview!$B$2</f>
         <v>84601628</v>
       </c>
       <c r="F11" s="18">
         <f t="shared" si="0"/>
         <v>4.683114372219882E-2</v>
+      </c>
+      <c r="G11" s="10">
+        <v>45915</v>
       </c>
     </row>
   </sheetData>
@@ -2844,7 +2820,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3272,8 +3248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5B1BD2-767A-46E8-A585-2C34077E3989}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3335,10 +3311,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF58C9D7-C19E-4761-9787-2A373F487714}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I1" sqref="I1:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3351,9 +3327,10 @@
     <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>92</v>
       </c>
@@ -3373,13 +3350,16 @@
         <v>101</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>45908</v>
       </c>
@@ -3399,15 +3379,18 @@
         <v>237</v>
       </c>
       <c r="G2" s="9">
-        <f>TwitterData_Stats!$B$2</f>
+        <f>Twitter_Overview!$B$2</f>
         <v>111878</v>
       </c>
       <c r="H2" s="11">
         <f>SUM(D2:F2)/G2</f>
         <v>0.64609664098392894</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>45908</v>
       </c>
@@ -3427,15 +3410,18 @@
         <v>864</v>
       </c>
       <c r="G3" s="9">
-        <f>TwitterData_Stats!$B$2</f>
+        <f>Twitter_Overview!$B$2</f>
         <v>111878</v>
       </c>
       <c r="H3" s="11">
         <f t="shared" ref="H3:H11" si="0">SUM(D3:F3)/G3</f>
         <v>1.1575555515829743</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>45908</v>
       </c>
@@ -3455,15 +3441,18 @@
         <v>255</v>
       </c>
       <c r="G4" s="9">
-        <f>TwitterData_Stats!$B$2</f>
+        <f>Twitter_Overview!$B$2</f>
         <v>111878</v>
       </c>
       <c r="H4" s="11">
         <f t="shared" si="0"/>
         <v>0.21510931550438872</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>45908</v>
       </c>
@@ -3483,15 +3472,18 @@
         <v>204</v>
       </c>
       <c r="G5" s="9">
-        <f>TwitterData_Stats!$B$2</f>
+        <f>Twitter_Overview!$B$2</f>
         <v>111878</v>
       </c>
       <c r="H5" s="11">
         <f t="shared" si="0"/>
         <v>0.25851373817908796</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>45908</v>
       </c>
@@ -3511,15 +3503,18 @@
         <v>269</v>
       </c>
       <c r="G6" s="9">
-        <f>TwitterData_Stats!$B$2</f>
+        <f>Twitter_Overview!$B$2</f>
         <v>111878</v>
       </c>
       <c r="H6" s="11">
         <f t="shared" si="0"/>
         <v>0.17081106204973273</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>45906</v>
       </c>
@@ -3539,15 +3534,18 @@
         <v>217</v>
       </c>
       <c r="G7" s="9">
-        <f>TwitterData_Stats!$B$2</f>
+        <f>Twitter_Overview!$B$2</f>
         <v>111878</v>
       </c>
       <c r="H7" s="11">
         <f t="shared" si="0"/>
         <v>0.13768569334453601</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>45906</v>
       </c>
@@ -3567,15 +3565,18 @@
         <v>332</v>
       </c>
       <c r="G8" s="9">
-        <f>TwitterData_Stats!$B$2</f>
+        <f>Twitter_Overview!$B$2</f>
         <v>111878</v>
       </c>
       <c r="H8" s="11">
         <f t="shared" si="0"/>
         <v>9.080426893580508E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>45905</v>
       </c>
@@ -3595,15 +3596,18 @@
         <v>174</v>
       </c>
       <c r="G9" s="9">
-        <f>TwitterData_Stats!$B$2</f>
+        <f>Twitter_Overview!$B$2</f>
         <v>111878</v>
       </c>
       <c r="H9" s="11">
         <f t="shared" si="0"/>
         <v>9.1188616171186468E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>45901</v>
       </c>
@@ -3623,15 +3627,18 @@
         <v>98</v>
       </c>
       <c r="G10" s="9">
-        <f>TwitterData_Stats!$B$2</f>
+        <f>Twitter_Overview!$B$2</f>
         <v>111878</v>
       </c>
       <c r="H10" s="11">
         <f t="shared" si="0"/>
         <v>9.2413164339727197E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>45897</v>
       </c>
@@ -3651,13 +3658,22 @@
         <v>172</v>
       </c>
       <c r="G11" s="9">
-        <f>TwitterData_Stats!$B$2</f>
+        <f>Twitter_Overview!$B$2</f>
         <v>111878</v>
       </c>
       <c r="H11" s="11">
         <f t="shared" si="0"/>
         <v>0.12552065642932481</v>
       </c>
+      <c r="I11" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="35"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3668,8 +3684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00D7A9F-20B8-4F57-A14E-BB573AD9F3F7}">
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5711,7 +5727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA86730-3D49-4594-85F8-2A1B87FD4262}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -6539,10 +6555,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179F9F10-530F-4257-B5F4-C178455903C0}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6551,9 +6567,10 @@
     <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>150</v>
       </c>
@@ -6566,8 +6583,11 @@
       <c r="D1" s="7" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="23">
         <f>ROW(A1)</f>
         <v>1</v>
@@ -6582,8 +6602,11 @@
       <c r="D2" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="23">
         <f t="shared" ref="A3:A33" si="0">ROW(A2)</f>
         <v>2</v>
@@ -6598,8 +6621,11 @@
       <c r="D3" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="23">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6614,8 +6640,11 @@
       <c r="D4" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="23">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6630,8 +6659,11 @@
       <c r="D5" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="23">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6646,8 +6678,11 @@
       <c r="D6" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="23">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6662,8 +6697,11 @@
       <c r="D7" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="23">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6678,8 +6716,11 @@
       <c r="D8" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6694,8 +6735,11 @@
       <c r="D9" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6710,8 +6754,11 @@
       <c r="D10" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6726,8 +6773,11 @@
       <c r="D11" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6742,8 +6792,11 @@
       <c r="D12" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6758,8 +6811,11 @@
       <c r="D13" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6774,8 +6830,11 @@
       <c r="D14" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -6790,8 +6849,11 @@
       <c r="D15" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -6806,8 +6868,11 @@
       <c r="D16" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -6822,8 +6887,11 @@
       <c r="D17" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6838,8 +6906,11 @@
       <c r="D18" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -6854,8 +6925,11 @@
       <c r="D19" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -6870,8 +6944,11 @@
       <c r="D20" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6886,8 +6963,11 @@
       <c r="D21" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -6902,8 +6982,11 @@
       <c r="D22" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -6918,8 +7001,11 @@
       <c r="D23" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -6934,8 +7020,11 @@
       <c r="D24" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -6950,8 +7039,11 @@
       <c r="D25" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="23">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -6966,8 +7058,11 @@
       <c r="D26" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="23">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -6982,8 +7077,11 @@
       <c r="D27" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="23">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -6998,8 +7096,11 @@
       <c r="D28" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="23">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -7014,8 +7115,11 @@
       <c r="D29" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="23">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -7030,8 +7134,11 @@
       <c r="D30" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="23">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7046,8 +7153,11 @@
       <c r="D31" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="23">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7062,8 +7172,11 @@
       <c r="D32" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="10">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="23">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7077,6 +7190,9 @@
       </c>
       <c r="D33" s="23">
         <v>0</v>
+      </c>
+      <c r="E33" s="10">
+        <v>45915</v>
       </c>
     </row>
   </sheetData>
@@ -7546,8 +7662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA47F01-DFB1-497B-A6BB-550548CE327E}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8068,7 +8184,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8089,7 +8205,7 @@
       <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="34"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -8128,7 +8244,7 @@
         <f>Summary!C15</f>
         <v>45920</v>
       </c>
-      <c r="D4" s="35"/>
+      <c r="D4" s="34"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -8163,10 +8279,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A73A83-EAE8-4493-85B3-97A94E227E50}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C18"/>
+      <selection activeCell="F1" sqref="F1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8176,9 +8292,10 @@
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>70</v>
       </c>
@@ -8194,8 +8311,11 @@
       <c r="E1" s="7" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>45</v>
       </c>
@@ -8211,8 +8331,11 @@
       <c r="E2" s="30">
         <v>0.14374999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>46</v>
       </c>
@@ -8228,8 +8351,11 @@
       <c r="E3" s="30">
         <v>0.11666666666666667</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>47</v>
       </c>
@@ -8245,8 +8371,11 @@
       <c r="E4" s="30">
         <v>0.1125</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
@@ -8262,8 +8391,11 @@
       <c r="E5" s="30">
         <v>0.11736111111111111</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>64</v>
       </c>
@@ -8279,8 +8411,11 @@
       <c r="E6" s="30">
         <v>0.10833333333333334</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>49</v>
       </c>
@@ -8296,8 +8431,11 @@
       <c r="E7" s="30">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>51</v>
       </c>
@@ -8313,8 +8451,11 @@
       <c r="E8" s="30">
         <v>0.16388888888888889</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>52</v>
       </c>
@@ -8330,8 +8471,11 @@
       <c r="E9" s="30">
         <v>0.17083333333333334</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>53</v>
       </c>
@@ -8347,8 +8491,11 @@
       <c r="E10" s="30">
         <v>0.14861111111111111</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>65</v>
       </c>
@@ -8364,8 +8511,11 @@
       <c r="E11" s="30">
         <v>9.2361111111111116E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>48</v>
       </c>
@@ -8381,8 +8531,11 @@
       <c r="E12" s="30">
         <v>0.10694444444444444</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>54</v>
       </c>
@@ -8398,8 +8551,11 @@
       <c r="E13" s="30">
         <v>0.11527777777777778</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>55</v>
       </c>
@@ -8415,8 +8571,11 @@
       <c r="E14" s="30">
         <v>9.7916666666666666E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>50</v>
       </c>
@@ -8432,8 +8591,11 @@
       <c r="E15" s="30">
         <v>0.11597222222222223</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>56</v>
       </c>
@@ -8449,8 +8611,11 @@
       <c r="E16" s="30">
         <v>0.12777777777777777</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>57</v>
       </c>
@@ -8466,8 +8631,11 @@
       <c r="E17" s="30">
         <v>0.12430555555555556</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>58</v>
       </c>
@@ -8482,6 +8650,9 @@
       </c>
       <c r="E18" s="30">
         <v>0.13125000000000001</v>
+      </c>
+      <c r="F18" s="10">
+        <v>45920</v>
       </c>
     </row>
   </sheetData>
@@ -8494,210 +8665,126 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA06E0B9-8043-46F5-ABCD-6F70405B8C26}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>158</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="29">
         <v>253078600</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
-        <v>47</v>
+      <c r="C2" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>62</v>
       </c>
       <c r="B3" s="29">
-        <v>253078600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>107388392</v>
+      </c>
+      <c r="C3" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B4" s="29">
-        <v>107388392</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
-        <v>57</v>
+        <v>979787719</v>
+      </c>
+      <c r="C4" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>61</v>
       </c>
       <c r="B5" s="29">
-        <v>107388392</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3085292140</v>
+      </c>
+      <c r="C5" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B6" s="29">
-        <v>979787719</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
-        <v>45</v>
+        <v>61804850</v>
+      </c>
+      <c r="C6" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>158</v>
       </c>
       <c r="B7" s="29">
-        <v>429228868</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="29">
-        <v>550558851</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="29">
-        <v>3085292140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="29">
-        <v>62453834</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="29">
-        <v>2000246989</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="29">
-        <v>33258008</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="29">
-        <v>39338067</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="29">
-        <v>101679472</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="29">
-        <v>67635844</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="29">
-        <v>34529394</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="29">
-        <v>251175060</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="29">
-        <v>70989383</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="29">
-        <v>40081478</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="29">
-        <v>322047684</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="29">
-        <v>61856927</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="29">
-        <v>61804850</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="29">
-        <v>61804850</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="B24" s="29">
         <v>4487351701</v>
       </c>
+      <c r="C7" s="35"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="35"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" s="35"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="35"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="35"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" s="35"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" s="35"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" s="35"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" s="35"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="35"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="35"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8709,7 +8796,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D18"/>
+      <selection activeCell="E11" sqref="E11:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8973,7 +9060,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9048,10 +9135,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0693C0-B4EA-4378-9A58-98E1E03D537E}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9060,9 +9147,10 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>72</v>
       </c>
@@ -9075,8 +9163,11 @@
       <c r="D1" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>45</v>
       </c>
@@ -9089,8 +9180,11 @@
       <c r="D2" s="9">
         <v>7789364</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>46</v>
       </c>
@@ -9103,8 +9197,11 @@
       <c r="D3" s="9">
         <v>11601066</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>19</v>
       </c>
@@ -9117,8 +9214,11 @@
       <c r="D4" s="9">
         <v>16858117</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>49</v>
       </c>
@@ -9131,8 +9231,11 @@
       <c r="D5" s="9">
         <v>2505794</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>64</v>
       </c>
@@ -9145,8 +9248,11 @@
       <c r="D6" s="9">
         <v>2523082</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>57</v>
       </c>
@@ -9159,8 +9265,11 @@
       <c r="D7" s="9">
         <v>1239856</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="10">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>58</v>
       </c>
@@ -9172,6 +9281,9 @@
       </c>
       <c r="D8" s="9">
         <v>508102</v>
+      </c>
+      <c r="E8" s="10">
+        <v>45920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>